<commit_message>
Update part descriptions. Change USB mini to micro.
</commit_message>
<xml_diff>
--- a/Manufacturing/BOM_ProgramingAddOn.xlsx
+++ b/Manufacturing/BOM_ProgramingAddOn.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brokebit/Sync/KiCad/ProgramingAddOn/Manufacturing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5EF2F439-B10B-6E42-AB85-D5D054915413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4F47F1A-05F6-4946-8FB9-519A81228D04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10880" yWindow="5640" windowWidth="27240" windowHeight="16440" xr2:uid="{84BDB74D-D6D4-B646-98BB-3E0D23FBE108}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{5CF2567F-2868-B044-9EBA-CA2E8F905839}" name="ProgramingAddOn" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/brokebit/Sync/KiCad/ProgramingAddOn/ProgramingAddOn.csv" tab="0" comma="1">
+    <textPr sourceFile="/Users/brokebit/Sync/KiCad/ProgramingAddOn/ProgramingAddOn.csv" tab="0" comma="1">
       <textFields count="7">
         <textField/>
         <textField/>
@@ -77,9 +77,6 @@
     <t>SW_DIP_x04</t>
   </si>
   <si>
-    <t>USB_B_Mini</t>
-  </si>
-  <si>
     <t>SW_DIP_x02</t>
   </si>
   <si>
@@ -158,9 +155,6 @@
     <t>Connector_USB:USB_Micro-B_Amphenol_10118194_Horizontal</t>
   </si>
   <si>
-    <t>USB Mini Type B connector</t>
-  </si>
-  <si>
     <t xml:space="preserve">J4, </t>
   </si>
   <si>
@@ -222,6 +216,12 @@
   </si>
   <si>
     <t>USB to UART master bridge, QFN-20</t>
+  </si>
+  <si>
+    <t>USB Micro Type B connector</t>
+  </si>
+  <si>
+    <t>USB_B_Micro</t>
   </si>
 </sst>
 </file>
@@ -580,7 +580,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -588,77 +588,77 @@
     <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.83203125" customWidth="1"/>
     <col min="3" max="4" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34.5" customWidth="1"/>
+    <col min="5" max="5" width="50.33203125" customWidth="1"/>
     <col min="6" max="6" width="80.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
         <v>15</v>
       </c>
-      <c r="E1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>16</v>
-      </c>
-      <c r="G1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2">
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
       </c>
       <c r="E2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" t="s">
         <v>20</v>
-      </c>
-      <c r="F2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D3" t="s">
         <v>1</v>
       </c>
       <c r="E3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" t="s">
         <v>20</v>
-      </c>
-      <c r="F3" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -670,115 +670,115 @@
         <v>4</v>
       </c>
       <c r="E4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" t="s">
         <v>25</v>
-      </c>
-      <c r="F4" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D5" t="s">
         <v>2</v>
       </c>
       <c r="E5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" t="s">
         <v>29</v>
-      </c>
-      <c r="F5" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>54</v>
       </c>
       <c r="D6" t="s">
-        <v>6</v>
+        <v>54</v>
       </c>
       <c r="E6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F6" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D9" t="s">
         <v>3</v>
       </c>
       <c r="E9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B10">
         <v>4</v>
@@ -790,35 +790,35 @@
         <v>3</v>
       </c>
       <c r="E10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B12">
         <v>4</v>
@@ -830,15 +830,15 @@
         <v>0</v>
       </c>
       <c r="E12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -850,30 +850,30 @@
         <v>5</v>
       </c>
       <c r="E13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>